<commit_message>
Credits for eelayed submissions of lab03
</commit_message>
<xml_diff>
--- a/lab/lab3/lab03_Section1.xlsx
+++ b/lab/lab3/lab03_Section1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liumanni/Documents/CSE 220/cse220_2020fall/lab/lab3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C53E0B9-A0B7-B540-8ABC-462846EF328E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C60F05D-5C15-EF40-B01E-3B6F4855D02F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{1C3543F5-1004-B644-A376-BBD6DC1ED258}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="49">
   <si>
     <t>Name</t>
   </si>
@@ -162,6 +162,24 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>Didn't attend the lab, didn't show TA the result. No longer on the D2L namelist.</t>
+  </si>
+  <si>
+    <t>Attended the lab, but didn't show TA the result. Responded on Piazza that he might use a "freebie" for this time.</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Attended the lab, but couldn't finish the two programs.</t>
+  </si>
+  <si>
+    <t>Delayed submission on Monday.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attended the lab, but didn't show TA the result. </t>
   </si>
 </sst>
 </file>
@@ -531,18 +549,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E6C37B7-F0BE-684B-BEEA-5AEE1918F2D1}">
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="106" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="106" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="4" max="4" width="40.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -553,7 +572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -564,7 +583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -575,12 +594,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -591,7 +619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -602,7 +630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -613,12 +641,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -629,7 +666,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -640,7 +677,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -651,7 +688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -662,7 +699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -673,7 +710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -684,7 +721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -695,7 +732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -706,12 +743,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -722,7 +768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -733,12 +779,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -749,17 +801,32 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -769,8 +836,11 @@
       <c r="C24">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -781,7 +851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -792,7 +862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -803,7 +873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -814,7 +884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -825,7 +895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -836,7 +906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -847,7 +917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -858,7 +928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -869,7 +939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -880,12 +950,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>41</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -896,7 +975,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -907,7 +986,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>38</v>
       </c>
@@ -918,7 +997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>39</v>
       </c>

</xml_diff>

<commit_message>
Minor changes to lab03 credit.
</commit_message>
<xml_diff>
--- a/lab/lab3/lab03_Section1.xlsx
+++ b/lab/lab3/lab03_Section1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liumanni/Documents/CSE 220/cse220_2020fall/lab/lab3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C60F05D-5C15-EF40-B01E-3B6F4855D02F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98184237-0CA5-F74C-B140-48E46850604C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{1C3543F5-1004-B644-A376-BBD6DC1ED258}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="50">
   <si>
     <t>Name</t>
   </si>
@@ -180,6 +180,9 @@
   </si>
   <si>
     <t xml:space="preserve">Attended the lab, but didn't show TA the result. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Didn't attend the lab, didn't show TA the result. </t>
   </si>
 </sst>
 </file>
@@ -551,8 +554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E6C37B7-F0BE-684B-BEEA-5AEE1918F2D1}">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="106" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="106" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -789,6 +792,9 @@
       <c r="C20">
         <v>0</v>
       </c>
+      <c r="D20" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
@@ -824,6 +830,9 @@
       </c>
       <c r="C23">
         <v>0</v>
+      </c>
+      <c r="D23" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>